<commit_message>
Updated filters for filtering down to 1000
</commit_message>
<xml_diff>
--- a/Criteria for ranking.xlsx
+++ b/Criteria for ranking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A23220E-D2A8-41A0-9178-CE5A231D7725}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875AD7DC-671D-41F8-A4C1-7594B248F124}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8925" xr2:uid="{C09B7413-CC9A-430D-973E-7141390B3386}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
   <si>
     <t>Criteria</t>
   </si>
@@ -157,6 +157,19 @@
 International Outlook: The ability of a university to attract undergraduates, postgraduates, and faculty from across the globe enhances its global standing.
 Financial Resources: The availability of financial resources for improving facilities, funding research, and supporting students is also a key factor.
 Alumni Success: The achievements of a university’s alumni, including awards, leadership positions, and contributions to their fields, reflect the institution’s impact on student’s career trajectories.</t>
+  </si>
+  <si>
+    <t>Carnegie Classification</t>
+  </si>
+  <si>
+    <t>carnegie_basic</t>
+  </si>
+  <si>
+    <t>1- Doctoral Universities: Very High Research Activity
+2- Doctoral Universities: High Research Activity
+3- Special Focus Four-Year: Research Institution
+4- Doctoral/Professional Universities
+5- Master’s Colleges &amp; Universities (Larger, Medium, Small Programs)</t>
   </si>
 </sst>
 </file>
@@ -211,9 +224,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -550,7 +566,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="B20" sqref="B20:G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,25 +581,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -654,7 +670,7 @@
       <c r="F5" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="3" t="s">
         <v>40</v>
       </c>
     </row>
@@ -671,7 +687,7 @@
       <c r="F6" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="3" t="s">
         <v>29</v>
       </c>
     </row>
@@ -679,6 +695,15 @@
       <c r="C7" t="s">
         <v>8</v>
       </c>
+      <c r="D7">
+        <v>120</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -700,12 +725,27 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9">
+        <v>120</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -797,62 +837,62 @@
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>